<commit_message>
Add shortcut to rename files/directories
</commit_message>
<xml_diff>
--- a/GitTerminalCmd.xlsx
+++ b/GitTerminalCmd.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alena\repos\CFG Autumn 25\test-repo1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alena\repos\CFG Autumn 25\Week1\Git-and-GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99F72BD-53C5-4E8D-A417-FE26114962BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC57C288-9C52-4D2A-8AD2-5DAE7F49A3FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="3000" windowWidth="18660" windowHeight="13725" activeTab="1" xr2:uid="{0DCA0E57-414C-4A57-8E97-43C142F07CC6}"/>
+    <workbookView xWindow="4995" yWindow="3900" windowWidth="18660" windowHeight="13725" activeTab="1" xr2:uid="{0DCA0E57-414C-4A57-8E97-43C142F07CC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Git Bash Commanda" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
   <si>
     <t>Command</t>
   </si>
@@ -305,6 +305,12 @@
   </si>
   <si>
     <t>back to root</t>
+  </si>
+  <si>
+    <t>mv old_file_name new_file_name</t>
+  </si>
+  <si>
+    <t>rename file/directory</t>
   </si>
 </sst>
 </file>
@@ -374,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -382,7 +388,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -773,7 +778,7 @@
       <c r="A6" s="2"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" t="s">
         <v>43</v>
       </c>
       <c r="B7" t="s">
@@ -781,7 +786,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
@@ -835,15 +840,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3210CDC2-59E1-4347-A714-6954E8224598}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="96.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -856,7 +861,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" t="s">
         <v>21</v>
       </c>
       <c r="B2" t="s">
@@ -864,7 +869,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" t="s">
         <v>23</v>
       </c>
       <c r="B3" t="s">
@@ -872,7 +877,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" t="s">
         <v>25</v>
       </c>
       <c r="B4" t="s">
@@ -880,7 +885,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -888,7 +893,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" t="s">
         <v>57</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -896,7 +901,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" t="s">
         <v>29</v>
       </c>
       <c r="B7" t="s">
@@ -904,7 +909,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" t="s">
         <v>31</v>
       </c>
       <c r="B8" t="s">
@@ -912,7 +917,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" t="s">
         <v>33</v>
       </c>
       <c r="B9" t="s">
@@ -920,7 +925,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" t="s">
         <v>35</v>
       </c>
       <c r="B10" t="s">
@@ -928,7 +933,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" t="s">
         <v>37</v>
       </c>
       <c r="B11" t="s">
@@ -936,7 +941,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" t="s">
         <v>39</v>
       </c>
       <c r="B12" t="s">
@@ -944,7 +949,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" t="s">
         <v>46</v>
       </c>
       <c r="B13" t="s">
@@ -952,7 +957,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" t="s">
         <v>48</v>
       </c>
       <c r="B14" t="s">
@@ -963,7 +968,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" t="s">
         <v>41</v>
       </c>
       <c r="B15" t="s">
@@ -971,7 +976,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" t="s">
         <v>51</v>
       </c>
       <c r="B16" t="s">
@@ -979,7 +984,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" t="s">
         <v>53</v>
       </c>
       <c r="B17" t="s">
@@ -987,11 +992,19 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" t="s">
         <v>56</v>
       </c>
       <c r="B18" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>